<commit_message>
updated. Grey literature included on sheets.
</commit_message>
<xml_diff>
--- a/data/exclude_list.xlsx
+++ b/data/exclude_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mflor\Documents\GitHub\dryland_restoration_synthesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455ED912-0113-43E0-9F79-A6DA97F929F1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1562CBD-AA0F-4E9F-A029-C37A8E53B453}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4070" xr2:uid="{C6F08BAA-C670-4BEE-8D8B-BC2F9FF4AD91}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3332" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3397" uniqueCount="976">
   <si>
     <t>ID</t>
   </si>
@@ -2880,6 +2880,87 @@
   </si>
   <si>
     <t>activities.aims.restortechnique</t>
+  </si>
+  <si>
+    <t>Atwell Island Restoration Project Activities 2000-2010</t>
+  </si>
+  <si>
+    <t>grey literature</t>
+  </si>
+  <si>
+    <t>rotational grazing</t>
+  </si>
+  <si>
+    <t>seeding, micro-topographic relief, fire, grazing</t>
+  </si>
+  <si>
+    <t>fallowing, disking, micro-topography</t>
+  </si>
+  <si>
+    <t>Central Valley Project Improvement Act Land Retirement Demonstration Project</t>
+  </si>
+  <si>
+    <t>retired croplands</t>
+  </si>
+  <si>
+    <t>salt-remediation products, seed coatings, and mycorrhizal inoculation</t>
+  </si>
+  <si>
+    <t>irrigation, planting, weed control</t>
+  </si>
+  <si>
+    <t>future strategy</t>
+  </si>
+  <si>
+    <t>Efficacy of habitat reclamation for endangered species at the Elk hills oil field, California</t>
+  </si>
+  <si>
+    <t>habitat for endangered species</t>
+  </si>
+  <si>
+    <t>oil and gas fields</t>
+  </si>
+  <si>
+    <t>ripped, disked</t>
+  </si>
+  <si>
+    <t>undisturbed sites</t>
+  </si>
+  <si>
+    <t>seeding, ripped, disked, fertilization</t>
+  </si>
+  <si>
+    <t>grey literature, success-costs</t>
+  </si>
+  <si>
+    <t>Restoration efforts of Atriplex canescens</t>
+  </si>
+  <si>
+    <t>grazing, seeding</t>
+  </si>
+  <si>
+    <t>native species</t>
+  </si>
+  <si>
+    <t>invasive species</t>
+  </si>
+  <si>
+    <t>native shrubland habitat</t>
+  </si>
+  <si>
+    <t>valley saltbush scrub community</t>
+  </si>
+  <si>
+    <t>seeding, tillage, weed suppression</t>
+  </si>
+  <si>
+    <t>tillage</t>
+  </si>
+  <si>
+    <t>solar power plant installation</t>
+  </si>
+  <si>
+    <t>California Valley Solar Ranch San Luis Obispo County, CA</t>
   </si>
 </sst>
 </file>
@@ -3250,11 +3331,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D62E3986-7054-4AE0-9A4D-11FC5C2A74FC}">
-  <dimension ref="A1:O274"/>
+  <dimension ref="A1:O279"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A268" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C284" sqref="C284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14628,6 +14709,226 @@
         <v>293</v>
       </c>
     </row>
+    <row r="275" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A275">
+        <v>274</v>
+      </c>
+      <c r="B275" t="s">
+        <v>949</v>
+      </c>
+      <c r="C275" t="s">
+        <v>952</v>
+      </c>
+      <c r="D275" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E275" t="s">
+        <v>76</v>
+      </c>
+      <c r="F275" t="s">
+        <v>4</v>
+      </c>
+      <c r="G275" t="s">
+        <v>293</v>
+      </c>
+      <c r="H275" t="s">
+        <v>950</v>
+      </c>
+      <c r="I275" t="s">
+        <v>758</v>
+      </c>
+      <c r="J275" t="s">
+        <v>951</v>
+      </c>
+      <c r="K275" t="s">
+        <v>348</v>
+      </c>
+      <c r="L275" t="s">
+        <v>953</v>
+      </c>
+      <c r="M275" t="s">
+        <v>348</v>
+      </c>
+      <c r="N275" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="276" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A276">
+        <v>275</v>
+      </c>
+      <c r="B276" t="s">
+        <v>954</v>
+      </c>
+      <c r="C276" t="s">
+        <v>957</v>
+      </c>
+      <c r="D276" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E276" t="s">
+        <v>76</v>
+      </c>
+      <c r="F276" t="s">
+        <v>4</v>
+      </c>
+      <c r="G276" t="s">
+        <v>293</v>
+      </c>
+      <c r="H276" t="s">
+        <v>950</v>
+      </c>
+      <c r="I276" t="s">
+        <v>955</v>
+      </c>
+      <c r="J276" t="s">
+        <v>958</v>
+      </c>
+      <c r="K276" t="s">
+        <v>348</v>
+      </c>
+      <c r="L276" t="s">
+        <v>956</v>
+      </c>
+      <c r="M276" t="s">
+        <v>348</v>
+      </c>
+      <c r="N276" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="277" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A277">
+        <v>276</v>
+      </c>
+      <c r="B277" t="s">
+        <v>959</v>
+      </c>
+      <c r="C277" t="s">
+        <v>964</v>
+      </c>
+      <c r="D277" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E277" t="s">
+        <v>76</v>
+      </c>
+      <c r="F277" t="s">
+        <v>4</v>
+      </c>
+      <c r="G277" t="s">
+        <v>293</v>
+      </c>
+      <c r="H277" t="s">
+        <v>965</v>
+      </c>
+      <c r="I277" t="s">
+        <v>961</v>
+      </c>
+      <c r="J277" t="s">
+        <v>4</v>
+      </c>
+      <c r="K277" t="s">
+        <v>960</v>
+      </c>
+      <c r="L277" t="s">
+        <v>962</v>
+      </c>
+      <c r="M277" t="s">
+        <v>963</v>
+      </c>
+      <c r="N277" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="278" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A278">
+        <v>277</v>
+      </c>
+      <c r="B278" t="s">
+        <v>966</v>
+      </c>
+      <c r="C278" t="s">
+        <v>967</v>
+      </c>
+      <c r="D278" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E278" t="s">
+        <v>76</v>
+      </c>
+      <c r="F278" t="s">
+        <v>4</v>
+      </c>
+      <c r="G278" t="s">
+        <v>293</v>
+      </c>
+      <c r="H278" t="s">
+        <v>950</v>
+      </c>
+      <c r="I278" t="s">
+        <v>969</v>
+      </c>
+      <c r="J278" t="s">
+        <v>803</v>
+      </c>
+      <c r="K278" t="s">
+        <v>968</v>
+      </c>
+      <c r="L278" t="s">
+        <v>4</v>
+      </c>
+      <c r="M278" t="s">
+        <v>333</v>
+      </c>
+      <c r="N278" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="279" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A279">
+        <v>278</v>
+      </c>
+      <c r="B279" t="s">
+        <v>975</v>
+      </c>
+      <c r="C279" t="s">
+        <v>972</v>
+      </c>
+      <c r="D279" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E279" t="s">
+        <v>76</v>
+      </c>
+      <c r="F279" t="s">
+        <v>4</v>
+      </c>
+      <c r="G279" t="s">
+        <v>293</v>
+      </c>
+      <c r="H279" t="s">
+        <v>950</v>
+      </c>
+      <c r="I279" t="s">
+        <v>974</v>
+      </c>
+      <c r="J279" t="s">
+        <v>704</v>
+      </c>
+      <c r="K279" t="s">
+        <v>970</v>
+      </c>
+      <c r="L279" t="s">
+        <v>973</v>
+      </c>
+      <c r="M279" t="s">
+        <v>971</v>
+      </c>
+      <c r="N279" t="s">
+        <v>733</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:N274" xr:uid="{C78D37E1-FDDF-4641-9FE4-8F903F4F0834}"/>
   <conditionalFormatting sqref="B1:B1048576">

</xml_diff>